<commit_message>
complete checklist with add country default
</commit_message>
<xml_diff>
--- a/чек лист формы обновление профиля.xlsx
+++ b/чек лист формы обновление профиля.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>№</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t xml:space="preserve">Поле окрашивается зеленым и заполняется выбранным сегментом бизнеса </t>
+  </si>
+  <si>
+    <t>Выбрать в поле   "Country"  страну по умолчанию (United States)</t>
   </si>
 </sst>
 </file>
@@ -530,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,26 +765,26 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -789,10 +792,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -800,10 +803,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -811,10 +814,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -822,7 +825,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>41</v>
@@ -833,10 +836,10 @@
         <v>26</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -844,10 +847,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -855,20 +858,31 @@
         <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C31" s="5" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>